<commit_message>
Empty cells return empty strings when :untyped
When running an :untyped spreadsheet import on xlsx files, Roo will now return an empty string.
</commit_message>
<xml_diff>
--- a/test/files/xlsx_test.xlsx
+++ b/test/files/xlsx_test.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="-440" yWindow="-19380" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
@@ -19,9 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -460,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -472,7 +475,7 @@
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" s="9">
         <v>1</v>
       </c>
@@ -506,8 +509,11 @@
       <c r="K1" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -515,7 +521,7 @@
         <v>41699</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>1.2</v>
       </c>
@@ -523,7 +529,7 @@
         <v>41699</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:13">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -531,7 +537,7 @@
         <v>41699</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:13">
       <c r="A5" s="4">
         <v>2122</v>
       </c>
@@ -539,27 +545,27 @@
         <v>41699</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:13">
       <c r="A6" s="6">
         <v>-23.000019999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:13">
       <c r="A7" s="8">
         <v>-23.000019999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:13">
       <c r="A8" s="7">
         <v>5.08</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:13">
       <c r="A10" s="2">
         <v>41677</v>
       </c>

</xml_diff>